<commit_message>
location bug issue and map updates
</commit_message>
<xml_diff>
--- a/ForecastedWeather.xlsx
+++ b/ForecastedWeather.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>

</xml_diff>

<commit_message>
Map prediction changes colour based on avg preipcover
</commit_message>
<xml_diff>
--- a/ForecastedWeather.xlsx
+++ b/ForecastedWeather.xlsx
@@ -468,12 +468,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>32</t>
+          <t>33</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>26</t>
+          <t>27</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -482,13 +482,13 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>1007</v>
+        <v>1006</v>
       </c>
       <c r="E2" t="n">
-        <v>25</v>
+        <v>66</v>
       </c>
       <c r="F2" t="n">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="3">
@@ -508,13 +508,13 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>1005</v>
+        <v>1007</v>
       </c>
       <c r="E3" t="n">
-        <v>66</v>
+        <v>25</v>
       </c>
       <c r="F3" t="n">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4">
@@ -525,7 +525,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>27</t>
+          <t>29</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -534,19 +534,19 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>1006</v>
+        <v>1008</v>
       </c>
       <c r="E4" t="n">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="F4" t="n">
-        <v>68</v>
+        <v>71</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>34</t>
+          <t>33</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -560,13 +560,13 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>1008</v>
+        <v>1007</v>
       </c>
       <c r="E5" t="n">
         <v>40</v>
       </c>
       <c r="F5" t="n">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="6">
@@ -577,7 +577,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>29</t>
+          <t>28</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -586,19 +586,19 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>1008</v>
+        <v>1006</v>
       </c>
       <c r="E6" t="n">
-        <v>40</v>
+        <v>71</v>
       </c>
       <c r="F6" t="n">
-        <v>76</v>
+        <v>79</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>33</t>
+          <t>32</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -612,24 +612,24 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>1007</v>
+        <v>1008</v>
       </c>
       <c r="E7" t="n">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="F7" t="n">
-        <v>74</v>
+        <v>79</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>33</t>
+          <t>34</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>28</t>
+          <t>25</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -638,13 +638,13 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>1008</v>
+        <v>1009</v>
       </c>
       <c r="E8" t="n">
-        <v>61</v>
+        <v>38</v>
       </c>
       <c r="F8" t="n">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>